<commit_message>
plot graph assignment 3
</commit_message>
<xml_diff>
--- a/Lectures and Assignment 2/problem3_Nguyen Xuan Binh_887799.xlsx
+++ b/Lectures and Assignment 2/problem3_Nguyen Xuan Binh_887799.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaltofi-my.sharepoint.com/personal/ilkka_j_leppanen_aalto_fi1/Documents/AALTO TEACHING/BUSINESS ANALYTICS 2 (2024)/assignment 2/answer templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\springnuance\Desktop\Business-Analytics-II\Lectures and Assignment 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{647C83F0-12BE-A149-8CBA-E5992BCE0A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F676587F-3FF8-BA4A-84F7-5F0BC8EF2F38}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43FE808-5FE1-449B-8C67-EDEB8881B4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1960" windowWidth="26840" windowHeight="14980" xr2:uid="{BBB29BED-96BF-5249-8910-3FADA7CE1B40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BBB29BED-96BF-5249-8910-3FADA7CE1B40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Cost of study</t>
   </si>
@@ -157,6 +157,30 @@
   <si>
     <t>Provide the answers in the green cell areas below. You can use any other areas in the worksheet to formulate calculations, draw the decision tree, and insert the graphs</t>
   </si>
+  <si>
+    <t>Profits (€M)</t>
+  </si>
+  <si>
+    <t>Own design</t>
+  </si>
+  <si>
+    <t>Licensing</t>
+  </si>
+  <si>
+    <t>s1: Low demand</t>
+  </si>
+  <si>
+    <t>–5</t>
+  </si>
+  <si>
+    <t>s2: Med demand</t>
+  </si>
+  <si>
+    <t>s3: High demand</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +189,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -218,8 +242,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF052025"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF052025"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +269,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -373,55 +416,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF98CA3E"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF98CA3E"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF98CA3E"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF98CA3E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -433,9 +490,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,6 +517,75 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>656493</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>146538</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>668215</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>5860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67C708AD-124A-9AF3-662E-E9A8254FC901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886093" y="7491046"/>
+          <a:ext cx="1201614" cy="457199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Decision: enter the market? </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-FI" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -750,371 +885,468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E02AD6-5D37-AA4E-8EB5-CBC2909E446C}">
-  <dimension ref="A2:G52"/>
+  <dimension ref="A2:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="21.69921875" customWidth="1"/>
+    <col min="3" max="3" width="13.69921875" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="14.796875" customWidth="1"/>
+    <col min="9" max="9" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="C7" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="D12" s="5">
+        <f>1-D5</f>
+        <v>0.95</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:D14" si="0">1-D6</f>
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="13" t="s">
+      <c r="C14" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="C18" s="13">
+        <v>0</v>
+      </c>
+      <c r="D18" s="13">
+        <v>-5</v>
+      </c>
+      <c r="E18" s="13">
+        <v>10</v>
+      </c>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="C19" s="13">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13">
+        <v>50</v>
+      </c>
+      <c r="E19" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
+      <c r="C20" s="13">
+        <v>0</v>
+      </c>
+      <c r="D20" s="13">
+        <v>120</v>
+      </c>
+      <c r="E20" s="13">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="B24" s="16"/>
+    </row>
+    <row r="25" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="19"/>
+      <c r="I25" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="I26" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="33">
+        <v>10</v>
+      </c>
+      <c r="L26" s="33">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I27" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" s="33">
+        <v>50</v>
+      </c>
+      <c r="K27" s="33">
+        <v>70</v>
+      </c>
+      <c r="L27" s="33">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="24"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="B28" s="23"/>
+      <c r="I28" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J28" s="33">
+        <v>120</v>
+      </c>
+      <c r="K28" s="33">
+        <v>90</v>
+      </c>
+      <c r="L28" s="33">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="24"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="B31" s="23"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="25"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="B34" s="24"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="26"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="B35" s="25"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="27"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="B36" s="26"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="24"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="B39" s="23"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="23"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="17"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="20"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="25"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="B45" s="24"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="27"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="B46" s="26"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="18"/>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="20"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="28"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="30"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="22"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="22"/>
-      <c r="G52" s="23"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="17"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="19"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="29"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="20"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>